<commit_message>
Automatische test-sync: 2025-08-08 20:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-08.xlsx
+++ b/logs/mail_log_2025-08-08.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -739,8 +739,61 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Zou jij dit even op kunnen pakken?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>"Testbedrijf 123 B.V." &lt;admin@testbedrijf123.nl&gt;</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Testmail #1: Zou jij dit even op kunnen pakken?
+Testbedrijf 123 B.V.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-08-08 19:59:52</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -760,7 +813,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -768,17 +821,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -793,7 +846,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -823,6 +876,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-08 20:01:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-08.xlsx
+++ b/logs/mail_log_2025-08-08.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -792,8 +792,61 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>"Testbedrijf 123 B.V." &lt;admin@testbedrijf123.nl&gt;</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?
+Testbedrijf 123 B.V.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-08-08 20:01:49</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -813,7 +866,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -821,17 +874,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -869,17 +922,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-08 20:11:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-08.xlsx
+++ b/logs/mail_log_2025-08-08.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -845,8 +845,61 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>"Testbedrijf 123 B.V." &lt;admin@testbedrijf123.nl&gt;</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?
+Testbedrijf 123 B.V.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-08-08 20:11:40</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -866,7 +919,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -874,17 +927,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -899,7 +952,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -939,6 +992,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-08 20:17:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-08.xlsx
+++ b/logs/mail_log_2025-08-08.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -898,8 +898,61 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>"Testbedrijf 123 B.V." &lt;admin@testbedrijf123.nl&gt;</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?
+Testbedrijf 123 B.V.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-08-08 20:16:50</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -919,7 +972,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -927,17 +980,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -985,17 +1038,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Intern verzoek / Actie voor medewerker</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>